<commit_message>
Colocando fontes no site
</commit_message>
<xml_diff>
--- a/Levantamento de dados/DadosCF (1).xlsx
+++ b/Levantamento de dados/DadosCF (1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\Plant.ai\Levantamento de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
   <si>
     <t>Tipos de plantas</t>
   </si>
@@ -206,6 +206,30 @@
   </si>
   <si>
     <t>Umidade Máxima</t>
+  </si>
+  <si>
+    <t>IDEAL</t>
+  </si>
+  <si>
+    <t>PLANTA EM RISCO</t>
+  </si>
+  <si>
+    <t>MUITO CALOR</t>
+  </si>
+  <si>
+    <t>MUITO FRIO</t>
+  </si>
+  <si>
+    <t>MUITA ÁGUA</t>
+  </si>
+  <si>
+    <t>POUCA ÁGUA</t>
+  </si>
+  <si>
+    <t>Temperatura (ºC)</t>
+  </si>
+  <si>
+    <t>Umidade (%)</t>
   </si>
 </sst>
 </file>
@@ -216,7 +240,7 @@
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,8 +267,68 @@
       <name val="Arial Rounded MT Bold"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14996795556505021"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Arial Rounded MT Bold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,8 +371,48 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0101"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -418,12 +542,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -467,13 +613,65 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="7" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="7" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="9">
+    <cellStyle name="Ênfase4" xfId="3" builtinId="41"/>
+    <cellStyle name="IDEAL" xfId="6"/>
+    <cellStyle name="MUITO CALOR" xfId="5"/>
+    <cellStyle name="MUITO FRIO" xfId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="RISCO CALOR" xfId="4"/>
+    <cellStyle name="RISCO FRIO" xfId="7"/>
+    <cellStyle name="Saída" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+      <color rgb="FFFF0101"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1406,19 +1604,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H16"/>
+  <dimension ref="A2:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H25" sqref="G25:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
     <col min="7" max="7" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1747,7 +1946,314 @@
         <v>80</v>
       </c>
     </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+    </row>
+    <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B27" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="38">
+        <v>10</v>
+      </c>
+      <c r="C28" s="39">
+        <f ca="1">_xlfn.QUARTILE.INC(B28:G28,1)</f>
+        <v>16</v>
+      </c>
+      <c r="D28" s="37">
+        <f ca="1">AVERAGE(B28:G28)</f>
+        <v>22</v>
+      </c>
+      <c r="E28" s="37">
+        <f ca="1">MEDIAN(B28:G28)</f>
+        <v>22</v>
+      </c>
+      <c r="F28" s="40">
+        <f ca="1">_xlfn.QUARTILE.INC(B28:G28,3)</f>
+        <v>28</v>
+      </c>
+      <c r="G28" s="41">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="38">
+        <v>9</v>
+      </c>
+      <c r="C29" s="39">
+        <f ca="1">_xlfn.QUARTILE.INC(B29:G29,1)</f>
+        <v>14.25</v>
+      </c>
+      <c r="D29" s="37">
+        <f ca="1">AVERAGE(B29:G29)</f>
+        <v>19.5</v>
+      </c>
+      <c r="E29" s="37">
+        <f ca="1">MEDIAN(B29:G29)</f>
+        <v>19.5</v>
+      </c>
+      <c r="F29" s="40">
+        <f ca="1">_xlfn.QUARTILE.INC(B29:G29,3)</f>
+        <v>24.75</v>
+      </c>
+      <c r="G29" s="41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="38">
+        <v>8</v>
+      </c>
+      <c r="C30" s="39">
+        <f ca="1">_xlfn.QUARTILE.INC(B30:G30,1)</f>
+        <v>12</v>
+      </c>
+      <c r="D30" s="37">
+        <f ca="1">AVERAGE(B30:G30)</f>
+        <v>16</v>
+      </c>
+      <c r="E30" s="37">
+        <f ca="1">MEDIAN(B30:G30)</f>
+        <v>16</v>
+      </c>
+      <c r="F30" s="40">
+        <f ca="1">_xlfn.QUARTILE.INC(B30:G30,3)</f>
+        <v>20</v>
+      </c>
+      <c r="G30" s="41">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="38">
+        <v>18</v>
+      </c>
+      <c r="C31" s="39">
+        <f ca="1">_xlfn.QUARTILE.INC(B31:G31,1)</f>
+        <v>22.25</v>
+      </c>
+      <c r="D31" s="37">
+        <f ca="1">AVERAGE(B31:G31)</f>
+        <v>26.5</v>
+      </c>
+      <c r="E31" s="37">
+        <f ca="1">MEDIAN(B31:G31)</f>
+        <v>26.5</v>
+      </c>
+      <c r="F31" s="40">
+        <f ca="1">_xlfn.QUARTILE.INC(B31:G31,3)</f>
+        <v>30.75</v>
+      </c>
+      <c r="G31" s="41">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="38">
+        <v>15</v>
+      </c>
+      <c r="C32" s="39">
+        <f ca="1">_xlfn.QUARTILE.INC(B32:G32,1)</f>
+        <v>20</v>
+      </c>
+      <c r="D32" s="37">
+        <f ca="1">AVERAGE(B32:G32)</f>
+        <v>25</v>
+      </c>
+      <c r="E32" s="37">
+        <f ca="1">MEDIAN(B32:G32)</f>
+        <v>25</v>
+      </c>
+      <c r="F32" s="40">
+        <f ca="1">_xlfn.QUARTILE.INC(B32:G32,3)</f>
+        <v>30</v>
+      </c>
+      <c r="G32" s="41">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+    </row>
+    <row r="39" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B39" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="G39" s="45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="35">
+        <v>60</v>
+      </c>
+      <c r="C40" s="49">
+        <f ca="1">_xlfn.QUARTILE.INC(B40:G40,1)</f>
+        <v>65</v>
+      </c>
+      <c r="D40" s="37">
+        <f ca="1">AVERAGE(B40:G40)</f>
+        <v>70</v>
+      </c>
+      <c r="E40" s="37">
+        <f ca="1">MEDIAN(B40:G40)</f>
+        <v>70</v>
+      </c>
+      <c r="F40" s="49">
+        <f ca="1">_xlfn.QUARTILE.INC(B40:G40,3)</f>
+        <v>75</v>
+      </c>
+      <c r="G40" s="41">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="35">
+        <v>60</v>
+      </c>
+      <c r="C41" s="49">
+        <f ca="1">_xlfn.QUARTILE.INC(B41:G41,1)</f>
+        <v>63.75</v>
+      </c>
+      <c r="D41" s="37">
+        <f ca="1">AVERAGE(B41:G41)</f>
+        <v>67.5</v>
+      </c>
+      <c r="E41" s="37">
+        <f ca="1">MEDIAN(B41:G41)</f>
+        <v>67.5</v>
+      </c>
+      <c r="F41" s="49">
+        <f ca="1">_xlfn.QUARTILE.INC(B41:G41,3)</f>
+        <v>71.25</v>
+      </c>
+      <c r="G41" s="41">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="35">
+        <v>80</v>
+      </c>
+      <c r="C42" s="49">
+        <f ca="1">_xlfn.QUARTILE.INC(B42:G42,1)</f>
+        <v>82</v>
+      </c>
+      <c r="D42" s="37">
+        <f ca="1">AVERAGE(B42:G42)</f>
+        <v>84</v>
+      </c>
+      <c r="E42" s="37">
+        <f ca="1">MEDIAN(B42:G42)</f>
+        <v>84</v>
+      </c>
+      <c r="F42" s="49">
+        <f ca="1">_xlfn.QUARTILE.INC(B42:G42,3)</f>
+        <v>86</v>
+      </c>
+      <c r="G42" s="41">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="35">
+        <v>60</v>
+      </c>
+      <c r="C43" s="49">
+        <f ca="1">_xlfn.QUARTILE.INC(B43:G43,1)</f>
+        <v>65</v>
+      </c>
+      <c r="D43" s="37">
+        <f ca="1">AVERAGE(B43:G43)</f>
+        <v>70</v>
+      </c>
+      <c r="E43" s="37">
+        <f ca="1">MEDIAN(B43:G43)</f>
+        <v>70</v>
+      </c>
+      <c r="F43" s="49">
+        <f ca="1">_xlfn.QUARTILE.INC(B43:G43,3)</f>
+        <v>75</v>
+      </c>
+      <c r="G43" s="41">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B38:G38"/>
+  </mergeCells>
   <conditionalFormatting sqref="H3">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>